<commit_message>
add hmm fusion algorithm in the main_offline.py file
</commit_message>
<xml_diff>
--- a/1-results/classification accuracy.xlsx
+++ b/1-results/classification accuracy.xlsx
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" activeCellId="1" sqref="J27:J31 J7:J11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,24 +1617,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="K2:K6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="K17:K21"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="K12:K16"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="J27:J31"/>
     <mergeCell ref="K27:K31"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="J22:J26"/>
     <mergeCell ref="K22:K26"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="K17:K21"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="J12:J16"/>
-    <mergeCell ref="K12:K16"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="K2:K6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="K7:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1643,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7:U7"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,11 +2646,11 @@
         <v>0.98245614035087703</v>
       </c>
       <c r="J27" s="7">
-        <f t="shared" ref="J27" si="8">AVERAGE(C27:I31)</f>
+        <f>AVERAGE(C27:I31)</f>
         <v>0.9640477963509414</v>
       </c>
       <c r="K27" s="7">
-        <f t="shared" ref="K27" si="9">_xlfn.STDEV.S(C27:I31)</f>
+        <f t="shared" ref="K27" si="8">_xlfn.STDEV.S(C27:I31)</f>
         <v>1.281975776906275E-2</v>
       </c>
     </row>
@@ -2770,26 +2770,72 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
     </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="K2:K6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="K17:K21"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="K12:K16"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="J27:J31"/>
     <mergeCell ref="K27:K31"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="J22:J26"/>
     <mergeCell ref="K22:K26"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="K17:K21"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="J12:J16"/>
-    <mergeCell ref="K12:K16"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="K2:K6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="K7:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>